<commit_message>
Summer 2023 Update fix
</commit_message>
<xml_diff>
--- a/Seasonal Anime Data/Summer 2023/Data Sheet.xlsx
+++ b/Seasonal Anime Data/Summer 2023/Data Sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="158">
   <si>
     <t>Title</t>
   </si>
@@ -31,6 +31,177 @@
     <t>link</t>
   </si>
   <si>
+    <t>BanG Dream! It's MyGO!!!!!</t>
+  </si>
+  <si>
+    <t>Jun 29</t>
+  </si>
+  <si>
+    <t>Jun 29, 2023</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/54959/BanG_Dream_Its_MyGO</t>
+  </si>
+  <si>
+    <t>Dungeon Meshi</t>
+  </si>
+  <si>
+    <t>Jul 1</t>
+  </si>
+  <si>
+    <t>Jul 1, 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comedy, Fantasy, Gourmet, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/52701/Dungeon_Meshi</t>
+  </si>
+  <si>
+    <t>Horimiya: Piece</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Romance, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/54856/Horimiya__Piece</t>
+  </si>
+  <si>
+    <t>Kage no Jitsuryokusha ni Naritakute! 2nd Season</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action, Comedy, Fantasy, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/54595/Kage_no_Jitsuryokusha_ni_Naritakute_2nd_Season</t>
+  </si>
+  <si>
+    <t>Jitsu wa Ore, Saikyou deshita?</t>
+  </si>
+  <si>
+    <t>Jul 2</t>
+  </si>
+  <si>
+    <t>Jul 2, 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adventure, Fantasy, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/52969/Jitsu_wa_Ore_Saikyou_deshita</t>
+  </si>
+  <si>
+    <t>Uchi no Kaisha no Chiisai Senpai no Hanashi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comedy, Romance, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/53379/Uchi_no_Kaisha_no_Chiisai_Senpai_no_Hanashi</t>
+  </si>
+  <si>
+    <t>Genjitsu no Yohane: Sunshine in the Mirror</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fantasy, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/52214/Genjitsu_no_Yohane__Sunshine_in_the_Mirror</t>
+  </si>
+  <si>
+    <t>Ayaka</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/53428/Ayaka</t>
+  </si>
+  <si>
+    <t>Ryza no Atelier: Tokoyami no Joou to Himitsu no Kakurega</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/54760/Ryza_no_Atelier__Tokoyami_no_Joou_to_Himitsu_no_Kakurega</t>
+  </si>
+  <si>
+    <t>Lv1 Maou to One Room Yuusha</t>
+  </si>
+  <si>
+    <t>Jul 3</t>
+  </si>
+  <si>
+    <t>Jul 3, 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comedy, Fantasy, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/51458/Lv1_Maou_to_One_Room_Yuusha</t>
+  </si>
+  <si>
+    <t>Masamune-kun no Revenge R</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/51498/Masamune-kun_no_Revenge_R</t>
+  </si>
+  <si>
+    <t>Mononogatari 2nd Season</t>
+  </si>
+  <si>
+    <t>Jul 4</t>
+  </si>
+  <si>
+    <t>Jul 4, 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action, Supernatural, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/54883/Mononogatari_2nd_Season</t>
+  </si>
+  <si>
+    <t>Suki na Ko ga Megane wo Wasureta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comedy, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/54234/Suki_na_Ko_ga_Megane_wo_Wasureta</t>
+  </si>
+  <si>
+    <t>Yumemiru Danshi wa Genjitsushugisha</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/53632/Yumemiru_Danshi_wa_Genjitsushugisha</t>
+  </si>
+  <si>
+    <t>Okashi na Tensei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fantasy, Gourmet, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/52611/Okashi_na_Tensei</t>
+  </si>
+  <si>
+    <t>Jidou Hanbaiki ni Umarekawatta Ore wa Meikyuu wo Samayou</t>
+  </si>
+  <si>
+    <t>Jul 5</t>
+  </si>
+  <si>
+    <t>Jul 5, 2023</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/52619/Jidou_Hanbaiki_ni_Umarekawatta_Ore_wa_Meikyuu_wo_Samayou</t>
+  </si>
+  <si>
+    <t>Watashi no Shiawase na Kekkon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fantasy, Romance, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/51552/Watashi_no_Shiawase_na_Kekkon</t>
+  </si>
+  <si>
     <t>Jujutsu Kaisen 2nd Season</t>
   </si>
   <si>
@@ -46,13 +217,187 @@
     <t>https://myanimelist.net/anime/51009/Jujutsu_Kaisen_2nd_Season</t>
   </si>
   <si>
+    <t>Undead Girl Murder Farce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mystery, Supernatural, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/54790/Undead_Girl_Murder_Farce</t>
+  </si>
+  <si>
+    <t>Seija Musou: Salaryman, Isekai de Ikinokoru Tame ni Ayumu Michi</t>
+  </si>
+  <si>
+    <t>Jul 7</t>
+  </si>
+  <si>
+    <t>Jul 7, 2023</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/53263/Seija_Musou__Salaryman_Isekai_de_Ikinokoru_Tame_ni_Ayumu_Michi</t>
+  </si>
+  <si>
+    <t>Hyakushou Kizoku</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/53426/Hyakushou_Kizoku</t>
+  </si>
+  <si>
+    <t>Sugar Apple Fairy Tale Part 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adventure, Fantasy, Romance, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/54842/Sugar_Apple_Fairy_Tale_Part_2</t>
+  </si>
+  <si>
+    <t>Higeki no Genkyou to Naru Saikyou Gedou Last Boss Joou wa Tami no Tame ni Tsukushimasu.</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/53438/Higeki_no_Genkyou_to_Naru_Saikyou_Gedou_Last_Boss_Joou_wa_Tami_no_Tame_ni_Tsukushimasu</t>
+  </si>
+  <si>
+    <t>Rurouni Kenshin: Meiji Kenkaku Romantan (2023)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action, Romance, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/50613/Rurouni_Kenshin__Meiji_Kenkaku_Romantan_2023</t>
+  </si>
+  <si>
+    <t>Shadowverse Flame: Seven Shadows-hen</t>
+  </si>
+  <si>
+    <t>Jul 8</t>
+  </si>
+  <si>
+    <t>Jul 8, 2023</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/54854/Shadowverse_Flame__Seven_Shadows-hen</t>
+  </si>
+  <si>
+    <t>AI no Idenshi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drama, Sci-Fi, Suspense, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/53787/AI_no_Idenshi</t>
+  </si>
+  <si>
+    <t>Ikimono-san</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avant Garde, Comedy, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/54847/Ikimono-san</t>
+  </si>
+  <si>
+    <t>Bleach: Sennen Kessen-hen - Ketsubetsu-tan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action, Adventure, Fantasy, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/53998/Bleach__Sennen_Kessen-hen_-_Ketsubetsu-tan</t>
+  </si>
+  <si>
+    <t>Kanojo, Okarishimasu 3rd Season</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/53050/Kanojo_Okarishimasu_3rd_Season</t>
+  </si>
+  <si>
+    <t>Dekiru Neko wa Kyou mo Yuuutsu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comedy, Supernatural, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/51916/Dekiru_Neko_wa_Kyou_mo_Yuuutsu</t>
+  </si>
+  <si>
+    <t>Liar Liar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecchi, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/48633/Liar_Liar</t>
+  </si>
+  <si>
+    <t>Nanatsu no Maken ga Shihai suru</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/50582/Nanatsu_no_Maken_ga_Shihai_suru</t>
+  </si>
+  <si>
+    <t>Cardfight!! Vanguard: will+Dress Season 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/52079/Cardfight_Vanguard__will_Dress_Season_3</t>
+  </si>
+  <si>
+    <t>Level 1 dakedo Unique Skill de Saikyou desu</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/51764/Level_1_dakedo_Unique_Skill_de_Saikyou_desu</t>
+  </si>
+  <si>
+    <t>Eiyuu Kyoushitsu</t>
+  </si>
+  <si>
+    <t>Jul 9</t>
+  </si>
+  <si>
+    <t>Jul 9, 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action, Fantasy, Ecchi, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/49894/Eiyuu_Kyoushitsu</t>
+  </si>
+  <si>
+    <t>Zom 100: Zombie ni Naru made ni Shitai 100 no Koto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action, Comedy, Horror, Supernatural, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/54112/Zom_100__Zombie_ni_Naru_made_ni_Shitai_100_no_Koto</t>
+  </si>
+  <si>
+    <t>Shinigami Bocchan to Kuro Maid 2nd Season</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/49858/Shinigami_Bocchan_to_Kuro_Maid_2nd_Season</t>
+  </si>
+  <si>
+    <t>Temple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comedy, Romance, Ecchi, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/54275/Temple</t>
+  </si>
+  <si>
     <t>Mushoku Tensei II: Isekai Ittara Honki Dasu</t>
   </si>
   <si>
-    <t>Jul 3</t>
-  </si>
-  <si>
-    <t>Jul 3, 2023</t>
+    <t>Jul 10</t>
+  </si>
+  <si>
+    <t>Jul 10, 2023</t>
   </si>
   <si>
     <t xml:space="preserve">Drama, Fantasy, Ecchi, </t>
@@ -61,96 +406,60 @@
     <t>https://myanimelist.net/anime/51179/Mushoku_Tensei_II__Isekai_Ittara_Honki_Dasu</t>
   </si>
   <si>
-    <t>Masamune-kun no Revenge R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comedy, Romance, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/51498/Masamune-kun_no_Revenge_R</t>
-  </si>
-  <si>
-    <t>Bleach: Sennen Kessen-hen - Ketsubetsu-tan</t>
-  </si>
-  <si>
-    <t>Jul 8</t>
-  </si>
-  <si>
-    <t>Jul 8, 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action, Adventure, Fantasy, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/53998/Bleach__Sennen_Kessen-hen_-_Ketsubetsu-tan</t>
-  </si>
-  <si>
-    <t>Horimiya: Piece</t>
-  </si>
-  <si>
-    <t>Jul 1</t>
-  </si>
-  <si>
-    <t>Jul 1, 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Romance, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/54856/Horimiya__Piece</t>
-  </si>
-  <si>
-    <t>Kanojo, Okarishimasu 3rd Season</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/53050/Kanojo_Okarishimasu_3rd_Season</t>
-  </si>
-  <si>
-    <t>Zom 100: Zombie ni Naru made ni Shitai 100 no Koto</t>
-  </si>
-  <si>
-    <t>Jul 9</t>
-  </si>
-  <si>
-    <t>Jul 9, 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action, Comedy, Horror, Supernatural, Suspense, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/54112/Zom_100__Zombie_ni_Naru_made_ni_Shitai_100_no_Koto</t>
+    <t>Dark Gathering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horror, Supernatural, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/52505/Dark_Gathering</t>
+  </si>
+  <si>
+    <t>Yami Shibai 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avant Garde, Horror, Supernatural, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/55166/Yami_Shibai_11</t>
+  </si>
+  <si>
+    <t>Synduality: Noir</t>
+  </si>
+  <si>
+    <t>Jul 11</t>
+  </si>
+  <si>
+    <t>Jul 11, 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sci-Fi, </t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/53026/Synduality__Noir</t>
+  </si>
+  <si>
+    <t>Helck</t>
+  </si>
+  <si>
+    <t>Jul 12</t>
+  </si>
+  <si>
+    <t>Jul 12, 2023</t>
+  </si>
+  <si>
+    <t>https://myanimelist.net/anime/51020/Helck</t>
   </si>
   <si>
     <t>Bungou Stray Dogs 5th Season</t>
   </si>
   <si>
-    <t>Jul 12</t>
-  </si>
-  <si>
-    <t>Jul 12, 2023</t>
-  </si>
-  <si>
     <t xml:space="preserve">Action, Mystery, Supernatural, </t>
   </si>
   <si>
     <t>https://myanimelist.net/anime/54898/Bungou_Stray_Dogs_5th_Season</t>
   </si>
   <si>
-    <t>Suki na Ko ga Megane wo Wasureta</t>
-  </si>
-  <si>
-    <t>Jul 4</t>
-  </si>
-  <si>
-    <t>Jul 4, 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comedy, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/54234/Suki_na_Ko_ga_Megane_wo_Wasureta</t>
-  </si>
-  <si>
     <t>Hataraku Maou-sama!! 2nd Season</t>
   </si>
   <si>
@@ -160,117 +469,9 @@
     <t>Jul 13, 2023</t>
   </si>
   <si>
-    <t xml:space="preserve">Comedy, Fantasy, </t>
-  </si>
-  <si>
     <t>https://myanimelist.net/anime/53200/Hataraku_Maou-sama_2nd_Season</t>
   </si>
   <si>
-    <t>Watashi no Shiawase na Kekkon</t>
-  </si>
-  <si>
-    <t>Jul 5</t>
-  </si>
-  <si>
-    <t>Jul 5, 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fantasy, Romance, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/51552/Watashi_no_Shiawase_na_Kekkon</t>
-  </si>
-  <si>
-    <t>Shinigami Bocchan to Kuro Maid 2nd Season</t>
-  </si>
-  <si>
-    <t>Jul 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comedy, Supernatural, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/49858/Shinigami_Bocchan_to_Kuro_Maid_2nd_Season</t>
-  </si>
-  <si>
-    <t>Liar Liar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ecchi, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/48633/Liar_Liar</t>
-  </si>
-  <si>
-    <t>Nanatsu no Maken ga Shihai suru</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/50582/Nanatsu_no_Maken_ga_Shihai_suru</t>
-  </si>
-  <si>
-    <t>Rurouni Kenshin: Meiji Kenkaku Romantan (2023)</t>
-  </si>
-  <si>
-    <t>Jul 7</t>
-  </si>
-  <si>
-    <t>Jul 7, 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action, Romance, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/50613/Rurouni_Kenshin__Meiji_Kenkaku_Romantan_2023</t>
-  </si>
-  <si>
-    <t>Eiyuu Kyoushitsu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action, Fantasy, Ecchi, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/49894/Eiyuu_Kyoushitsu</t>
-  </si>
-  <si>
-    <t>Uchi no Kaisha no Chiisai Senpai no Hanashi</t>
-  </si>
-  <si>
-    <t>Jul 2</t>
-  </si>
-  <si>
-    <t>Jul 2, 2023</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/53379/Uchi_no_Kaisha_no_Chiisai_Senpai_no_Hanashi</t>
-  </si>
-  <si>
-    <t>Yumemiru Danshi wa Genjitsushugisha</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/53632/Yumemiru_Danshi_wa_Genjitsushugisha</t>
-  </si>
-  <si>
-    <t>Jidou Hanbaiki ni Umarekawatta Ore wa Meikyuu wo Samayou</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/52619/Jidou_Hanbaiki_ni_Umarekawatta_Ore_wa_Meikyuu_wo_Samayou</t>
-  </si>
-  <si>
-    <t>Dark Gathering</t>
-  </si>
-  <si>
-    <t>Jul 10</t>
-  </si>
-  <si>
-    <t>Jul 10, 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horror, Supernatural, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/52505/Dark_Gathering</t>
-  </si>
-  <si>
     <t>Shiro Seijo to Kuro Bokushi</t>
   </si>
   <si>
@@ -280,111 +481,6 @@
     <t>https://myanimelist.net/anime/52082/Shiro_Seijo_to_Kuro_Bokushi</t>
   </si>
   <si>
-    <t>Jitsu wa Ore, Saikyou deshita?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adventure, Fantasy, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/52969/Jitsu_wa_Ore_Saikyou_deshita</t>
-  </si>
-  <si>
-    <t>Level 1 dakedo Unique Skill de Saikyou desu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fantasy, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/51764/Level_1_dakedo_Unique_Skill_de_Saikyou_desu</t>
-  </si>
-  <si>
-    <t>Sugar Apple Fairy Tale Part 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adventure, Fantasy, Romance, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/54842/Sugar_Apple_Fairy_Tale_Part_2</t>
-  </si>
-  <si>
-    <t>Higeki no Genkyou to Naru Saikyou Gedou Last Boss Joou wa Tami no Tame ni Tsukushimasu.</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/53438/Higeki_no_Genkyou_to_Naru_Saikyou_Gedou_Last_Boss_Joou_wa_Tami_no_Tame_ni_Tsukushimasu</t>
-  </si>
-  <si>
-    <t>Ryza no Atelier: Tokoyami no Joou to Himitsu no Kakurega</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/54760/Ryza_no_Atelier__Tokoyami_no_Joou_to_Himitsu_no_Kakurega</t>
-  </si>
-  <si>
-    <t>Helck</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/51020/Helck</t>
-  </si>
-  <si>
-    <t>Undead Girl Murder Farce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mystery, Supernatural, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/54790/Undead_Girl_Murder_Farce</t>
-  </si>
-  <si>
-    <t>Temple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comedy, Romance, Ecchi, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/54275/Temple</t>
-  </si>
-  <si>
-    <t>Dekiru Neko wa Kyou mo Yuuutsu</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/51916/Dekiru_Neko_wa_Kyou_mo_Yuuutsu</t>
-  </si>
-  <si>
-    <t>Genjitsu no Yohane: Sunshine in the Mirror</t>
-  </si>
-  <si>
-    <t>Jun 25</t>
-  </si>
-  <si>
-    <t>Jun 25, 2023</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/52214/Genjitsu_no_Yohane__Sunshine_in_the_Mirror</t>
-  </si>
-  <si>
-    <t>Seija Musou: Salaryman, Isekai de Ikinokoru Tame ni Ayumu Michi</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/53263/Seija_Musou__Salaryman_Isekai_de_Ikinokoru_Tame_ni_Ayumu_Michi</t>
-  </si>
-  <si>
-    <t>AI no Idenshi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drama, Sci-Fi, Suspense, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/53787/AI_no_Idenshi</t>
-  </si>
-  <si>
-    <t>Okashi na Tensei</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fantasy, Gourmet, Slice of Life, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/52611/Okashi_na_Tensei</t>
-  </si>
-  <si>
     <t>Spy Kyoushitsu 2nd Season</t>
   </si>
   <si>
@@ -392,93 +488,6 @@
   </si>
   <si>
     <t>https://myanimelist.net/anime/54947/Spy_Kyoushitsu_2nd_Season</t>
-  </si>
-  <si>
-    <t>Mononogatari 2nd Season</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action, Supernatural, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/54883/Mononogatari_2nd_Season</t>
-  </si>
-  <si>
-    <t>Ayaka</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/53428/Ayaka</t>
-  </si>
-  <si>
-    <t>Lv1 Maou to One Room Yuusha</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/51458/Lv1_Maou_to_One_Room_Yuusha</t>
-  </si>
-  <si>
-    <t>Synduality: Noir</t>
-  </si>
-  <si>
-    <t>Jul 11</t>
-  </si>
-  <si>
-    <t>Jul 11, 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sci-Fi, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/53026/Synduality__Noir</t>
-  </si>
-  <si>
-    <t>BanG Dream! It's MyGO!!!!!</t>
-  </si>
-  <si>
-    <t>Jun 29</t>
-  </si>
-  <si>
-    <t>Jun 29, 2023</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/54959/BanG_Dream_Its_MyGO</t>
-  </si>
-  <si>
-    <t>Yami Shibai 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avant Garde, Horror, Supernatural, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/55166/Yami_Shibai_11</t>
-  </si>
-  <si>
-    <t>Hyakushou Kizoku</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/53426/Hyakushou_Kizoku</t>
-  </si>
-  <si>
-    <t>Cardfight!! Vanguard: will+Dress Season 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/52079/Cardfight_Vanguard__will_Dress_Season_3</t>
-  </si>
-  <si>
-    <t>Shadowverse Flame: Seven Shadows-hen</t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/54854/Shadowverse_Flame__Seven_Shadows-hen</t>
-  </si>
-  <si>
-    <t>Ikimono-san</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avant Garde, Comedy, </t>
-  </si>
-  <si>
-    <t>https://myanimelist.net/anime/54847/Ikimono-san</t>
   </si>
 </sst>
 </file>
@@ -823,7 +832,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C2:G47"/>
+  <dimension ref="C2:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -856,756 +865,790 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="3:7">
       <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="3:7">
       <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="3:7">
       <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="3:7">
       <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="3:7">
       <c r="C8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="3:7">
       <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="3:7">
       <c r="C10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="3:7">
       <c r="C11" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="3:7">
       <c r="C12" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="3:7">
       <c r="C13" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="3:7">
       <c r="C14" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="3:7">
       <c r="C15" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="3:7">
       <c r="C16" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="3:7">
       <c r="C17" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="3:7">
       <c r="C18" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="3:7">
       <c r="C19" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="F19" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="3:7">
       <c r="C20" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="F20" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="3:7">
       <c r="C21" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="F21" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="3:7">
       <c r="C22" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E22" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F22" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="3:7">
       <c r="C23" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="F23" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="3:7">
       <c r="C24" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F24" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="3:7">
       <c r="C25" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="E25" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="F25" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="3:7">
       <c r="C26" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E26" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F26" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="3:7">
       <c r="C27" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="E27" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="F27" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="3:7">
       <c r="C28" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="E28" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="F28" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="3:7">
       <c r="C29" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="E29" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="F29" t="s">
-        <v>8</v>
+        <v>92</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="3:7">
       <c r="C30" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="E30" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="F30" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="3:7">
       <c r="C31" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="E31" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="F31" t="s">
-        <v>107</v>
+        <v>26</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="3:7">
       <c r="C32" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D32" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="E32" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="F32" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="3:7">
       <c r="C33" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D33" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="E33" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="F33" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="3:7">
       <c r="C34" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D34" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" t="s">
         <v>65</v>
       </c>
-      <c r="E34" t="s">
-        <v>66</v>
-      </c>
-      <c r="F34" t="s">
-        <v>92</v>
-      </c>
       <c r="G34" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="3:7">
       <c r="C35" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="D35" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="E35" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="F35" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="3:7">
       <c r="C36" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="E36" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="F36" t="s">
-        <v>121</v>
+        <v>29</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="3:7">
       <c r="C37" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D37" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
       <c r="E37" t="s">
-        <v>56</v>
+        <v>114</v>
       </c>
       <c r="F37" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="3:7">
       <c r="C38" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="D38" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="E38" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
       <c r="F38" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="3:7">
       <c r="C39" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D39" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="E39" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="F39" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="3:7">
       <c r="C40" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D40" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="E40" t="s">
-        <v>25</v>
+        <v>114</v>
       </c>
       <c r="F40" t="s">
-        <v>48</v>
+        <v>123</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="3:7">
       <c r="C41" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D41" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E41" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F41" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="3:7">
       <c r="C42" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D42" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="E42" t="s">
-        <v>140</v>
+        <v>127</v>
+      </c>
+      <c r="F42" t="s">
+        <v>131</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="3:7">
       <c r="C43" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D43" t="s">
-        <v>56</v>
+        <v>126</v>
       </c>
       <c r="E43" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
       <c r="F43" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="3:7">
       <c r="C44" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D44" t="s">
-        <v>65</v>
+        <v>137</v>
       </c>
       <c r="E44" t="s">
-        <v>66</v>
+        <v>138</v>
       </c>
       <c r="F44" t="s">
-        <v>43</v>
+        <v>139</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="3:7">
       <c r="C45" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D45" t="s">
-        <v>19</v>
+        <v>142</v>
       </c>
       <c r="E45" t="s">
-        <v>20</v>
+        <v>143</v>
       </c>
       <c r="F45" t="s">
-        <v>148</v>
+        <v>65</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="3:7">
       <c r="C46" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D46" t="s">
-        <v>19</v>
+        <v>142</v>
       </c>
       <c r="E46" t="s">
-        <v>20</v>
+        <v>143</v>
       </c>
       <c r="F46" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="47" spans="3:7">
       <c r="C47" t="s">
+        <v>148</v>
+      </c>
+      <c r="D47" t="s">
+        <v>149</v>
+      </c>
+      <c r="E47" t="s">
+        <v>150</v>
+      </c>
+      <c r="F47" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7">
+      <c r="C48" t="s">
         <v>152</v>
       </c>
-      <c r="D47" t="s">
-        <v>19</v>
-      </c>
-      <c r="E47" t="s">
-        <v>20</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="D48" t="s">
+        <v>149</v>
+      </c>
+      <c r="E48" t="s">
+        <v>150</v>
+      </c>
+      <c r="F48" t="s">
         <v>153</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>154</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7">
+      <c r="C49" t="s">
+        <v>155</v>
+      </c>
+      <c r="D49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E49" t="s">
+        <v>150</v>
+      </c>
+      <c r="F49" t="s">
+        <v>156</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1655,6 +1698,8 @@
     <hyperlink ref="G45" r:id="rId43"/>
     <hyperlink ref="G46" r:id="rId44"/>
     <hyperlink ref="G47" r:id="rId45"/>
+    <hyperlink ref="G48" r:id="rId46"/>
+    <hyperlink ref="G49" r:id="rId47"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>